<commit_message>
messy code but the bot is able to iterate through the first five comments of each post.
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -1,73 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanshu\Desktop\Repo\Python-RedditBot-Collab\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F87CF3-90A2-4ABC-B947-E8EF1A5D0AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>I took this from the passenger seat of a moving vehicle in Glacier National Park [5499x3093][OC]</t>
-  </si>
-  <si>
-    <t>Hey Reddit! We are Nimble Giant, an indie studio developing Quantum League, a first person shooter with an unique time-loop mechanic that allows you to team up with yourself. Check the game on Steam and make sure to wishlist!</t>
-  </si>
-  <si>
-    <t>Maui, Hawai’i [4376 x 3501] [OC]</t>
-  </si>
-  <si>
-    <t>Four years ago at Grand Teton National Park! Living vicariously through old photos until things improve [OC][3270x4087] | Insta: @pixelsdisclosed</t>
-  </si>
-  <si>
-    <t>Two years ago I saw this sunrise, the best I've seen still to this day. The park is closed now, but I'm desperately awaiting the day we can get back outside and enjoy our natural areas again. Glacier National Park, MT [OC][1278x19200]</t>
-  </si>
-  <si>
-    <t>IMPORTANT PSA: No, you did not win a gift card.</t>
-  </si>
-  <si>
-    <t>Eminem Donated Spaghetti Cups to DMC Hospital Healthcare Workers in Detroit Tonight</t>
-  </si>
-  <si>
-    <t>A buck with a crown of leaves</t>
-  </si>
-  <si>
-    <t>What a trippy tattoo</t>
-  </si>
-  <si>
-    <t>Lad wrote a Python script to download Alexa voice recordings, he didn't expect this email.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -86,21 +46,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -366,95 +317,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="208.5703125" customWidth="1"/>
+    <col width="208.5703125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>I took this from the passenger seat of a moving vehicle in Glacier National Park [5499x3093][OC]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Hey Reddit! We are Nimble Giant, an indie studio developing Quantum League, a first person shooter with an unique time-loop mechanic that allows you to team up with yourself. Check the game on Steam and make sure to wishlist!</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Maui, Hawai’i [4376 x 3501] [OC]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Four years ago at Grand Teton National Park! Living vicariously through old photos until things improve [OC][3270x4087] | Insta: @pixelsdisclosed</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Two years ago I saw this sunrise, the best I've seen still to this day. The park is closed now, but I'm desperately awaiting the day we can get back outside and enjoy our natural areas again. Glacier National Park, MT [OC][1278x19200]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IMPORTANT PSA: No, you did not win a gift card.</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eminem Donated Spaghetti Cups to DMC Hospital Healthcare Workers in Detroit Tonight</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A buck with a crown of leaves</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>What a trippy tattoo</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lad wrote a Python script to download Alexa voice recordings, he didn't expect this email.</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hanging Lake, Colorado [2932 x 2347] [OC]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Color reflections near Palmer, Alaska [1080x1280] OC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Counter-Protester steals show from Idiots</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>I'm starting a sofa counter-protest #StayAtHome</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lake Louise {2436x1125} {OC}</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Grand Canyon - Deer Creek [2600 × 3920] [OC]</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Waimea Canyon, Kauai, Hawaii, USA [OC][2000x3000]</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>During a protest in Arizona three nurses showed up to counter-protest the Liberate Rally.</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>25 bags of trash cleaned up today. #trashtag</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Recreation of "Dr Samuel Johnson" by Sir Joshua Reynolds (1772/1775)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>My Professor wants hand written assignments. So I made MyhandWriting.. that can write in myway on a A4 sheet paper.</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
module 5 post upvote integration
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Python-RedditBot-Collab\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D83335F-F3D3-425E-91E1-757CEFFCDD71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,12 +55,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -317,230 +335,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="208.5703125" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="208.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>I took this from the passenger seat of a moving vehicle in Glacier National Park [5499x3093][OC]</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hey Reddit! We are Nimble Giant, an indie studio developing Quantum League, a first person shooter with an unique time-loop mechanic that allows you to team up with yourself. Check the game on Steam and make sure to wishlist!</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Maui, Hawai’i [4376 x 3501] [OC]</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Four years ago at Grand Teton National Park! Living vicariously through old photos until things improve [OC][3270x4087] | Insta: @pixelsdisclosed</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Two years ago I saw this sunrise, the best I've seen still to this day. The park is closed now, but I'm desperately awaiting the day we can get back outside and enjoy our natural areas again. Glacier National Park, MT [OC][1278x19200]</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>IMPORTANT PSA: No, you did not win a gift card.</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Eminem Donated Spaghetti Cups to DMC Hospital Healthcare Workers in Detroit Tonight</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>A buck with a crown of leaves</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>What a trippy tattoo</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Lad wrote a Python script to download Alexa voice recordings, he didn't expect this email.</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Hanging Lake, Colorado [2932 x 2347] [OC]</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Color reflections near Palmer, Alaska [1080x1280] OC</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Counter-Protester steals show from Idiots</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>I'm starting a sofa counter-protest #StayAtHome</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Lake Louise {2436x1125} {OC}</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Grand Canyon - Deer Creek [2600 × 3920] [OC]</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Waimea Canyon, Kauai, Hawaii, USA [OC][2000x3000]</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>During a protest in Arizona three nurses showed up to counter-protest the Liberate Rally.</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>25 bags of trash cleaned up today. #trashtag</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Recreation of "Dr Samuel Johnson" by Sir Joshua Reynolds (1772/1775)</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>My Professor wants hand written assignments. So I made MyhandWriting.. that can write in myway on a A4 sheet paper.</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Module 5 && Module 4 clean up
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -322,148 +322,82 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A23:A28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="208.5703125" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>/r/EarthPorn/comments/g7nxna/northern_lights_dancing_over_the_tailrace_in/</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>/r/EarthPorn/comments/g7soyl/spooky_fog_during_hike_to_kendall_knob_washington/</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>/r/goodnews/comments/fk33b0/modmessage_visit_the_good_news_discord_server/</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>/r/goodnews/comments/g783r7/good_news_its_friday_whats_your_feelgood_story/</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/r/learnpython/comments/g4iiwc/ask_anything_monday_weekly_thread/</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/r/learnpython/comments/g7rpwu/ok_so_im_committed_to_1_year_of_coding_in_python/</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/r/pics/comments/fjn0j9/important_psa_no_you_did_not_win_a_gift_card/</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>0</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/r/pics/comments/g7rlvg/when_a_cat_runs_to_the_fridge_every_time_it_opens/</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>0</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/r/Python/comments/g5fwr9/whats_everyone_working_on_this_week/</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>/r/EarthPorn/comments/g72zis/insane_color_palette_in_chickaloon_alaska/</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>/r/pics/comments/fjn0j9/important_psa_no_you_did_not_win_a_gift_card/</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>/r/pics/comments/g76zbc/out_for_my_daily_walk/</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>/r/Python/comments/g78ih1/i_wrote_a_program_on_python_to_show_how_the/</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/r/Python/comments/g7q2ej/my_pothole_detector_used_yolov3_annotated_images/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
post upvote testing 6/21/20
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I50" sqref="I50"/>
@@ -401,6 +401,90 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/r/EarthPorn/comments/gz78ba/open_letter_to_steve_huffman_and_the_board_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/r/EarthPorn/comments/hd5a2q/seascape_sunset_at_the_cliff_in_sydney_australia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/r/goodnews/comments/gwtp43/whats_new_content_creators_june_2020/</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/r/goodnews/comments/hc0d3l/good_news_its_friday_whats_your_feelgood_story/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/r/learnpython/comments/h9527c/ask_anything_monday_weekly_thread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>/r/learnpython/comments/hd6uou/book_recommendations_taking_udemy_course_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>/r/pics/comments/hd8660/michael_and_barbara_shetterly_listen_to_their_son/</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>/r/Python/comments/gdfaip/rpython_job_board_for_may_june_july/</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>/r/Python/comments/ha4qfy/whats_everyone_working_on_this_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>/r/EarthPorn/comments/hdd0k7/anyone_else_need_some_color_today_little_ohio/</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>/r/learnpython/comments/hd9oaf/what_are_some_really_introbeginner_basic_project/</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>/r/pics/comments/hda7w3/dubai_solar_eclipse_by_josh_cripps/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test run to spot bugs for squashing
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -322,10 +322,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -334,42 +334,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/r/EarthPorn/comments/g7nxna/northern_lights_dancing_over_the_tailrace_in/</t>
+          <t>/r/EarthPorn/comments/gz78ba/open_letter_to_steve_huffman_and_the_board_of/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/r/EarthPorn/comments/g7soyl/spooky_fog_during_hike_to_kendall_knob_washington/</t>
+          <t>/r/EarthPorn/comments/hdsj7b/tried_to_find_a_leprechauns_pot_of_gold_but_got/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/r/goodnews/comments/fk33b0/modmessage_visit_the_good_news_discord_server/</t>
+          <t>/r/goodnews/comments/gwtp43/whats_new_content_creators_june_2020/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/r/goodnews/comments/g783r7/good_news_its_friday_whats_your_feelgood_story/</t>
+          <t>/r/goodnews/comments/hc0d3l/good_news_its_friday_whats_your_feelgood_story/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/r/learnpython/comments/g4iiwc/ask_anything_monday_weekly_thread/</t>
+          <t>/r/learnpython/comments/hdhm9j/ask_anything_monday_weekly_thread/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/r/learnpython/comments/g7rpwu/ok_so_im_committed_to_1_year_of_coding_in_python/</t>
+          <t>/r/learnpython/comments/hduh6k/how_to_approach_automate_the_boring_stuff/</t>
         </is>
       </c>
     </row>
@@ -383,105 +383,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>/r/pics/comments/g7rlvg/when_a_cat_runs_to_the_fridge_every_time_it_opens/</t>
+          <t>/r/pics/comments/hdyxvr/bubba_wallace_nascars_only_black_driver_with/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>/r/Python/comments/g5fwr9/whats_everyone_working_on_this_week/</t>
+          <t>/r/Python/comments/gdfaip/rpython_job_board_for_may_june_july/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>/r/Python/comments/g7q2ej/my_pothole_detector_used_yolov3_annotated_images/</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>/r/EarthPorn/comments/gz78ba/open_letter_to_steve_huffman_and_the_board_of/</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>/r/EarthPorn/comments/hd5a2q/seascape_sunset_at_the_cliff_in_sydney_australia/</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>/r/goodnews/comments/gwtp43/whats_new_content_creators_june_2020/</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>/r/goodnews/comments/hc0d3l/good_news_its_friday_whats_your_feelgood_story/</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>/r/learnpython/comments/h9527c/ask_anything_monday_weekly_thread/</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>/r/learnpython/comments/hd6uou/book_recommendations_taking_udemy_course_and/</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>/r/pics/comments/hd8660/michael_and_barbara_shetterly_listen_to_their_son/</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>/r/Python/comments/gdfaip/rpython_job_board_for_may_june_july/</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
           <t>/r/Python/comments/ha4qfy/whats_everyone_working_on_this_week/</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>/r/EarthPorn/comments/hdd0k7/anyone_else_need_some_color_today_little_ohio/</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>/r/learnpython/comments/hd9oaf/what_are_some_really_introbeginner_basic_project/</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>/r/pics/comments/hda7w3/dubai_solar_eclipse_by_josh_cripps/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
file names optimized and upvote button fixed
</commit_message>
<xml_diff>
--- a/reddit_posts.xlsx
+++ b/reddit_posts.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -325,7 +325,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A1048576"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -341,35 +341,35 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/r/EarthPorn/comments/hdsj7b/tried_to_find_a_leprechauns_pot_of_gold_but_got/</t>
+          <t>/r/EarthPorn/comments/hhxc58/oc_amazing_sunset_colours_and_swell_in_south/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/r/goodnews/comments/gwtp43/whats_new_content_creators_june_2020/</t>
+          <t>/r/learnpython/comments/hhpl9c/ask_anything_monday_weekly_thread/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/r/goodnews/comments/hc0d3l/good_news_its_friday_whats_your_feelgood_story/</t>
+          <t>/r/goodnews/comments/gwtp43/whats_new_content_creators_june_2020/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/r/learnpython/comments/hdhm9j/ask_anything_monday_weekly_thread/</t>
+          <t>/r/goodnews/comments/hg7813/good_news_its_friday_whats_your_feelgood_story/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/r/learnpython/comments/hduh6k/how_to_approach_automate_the_boring_stuff/</t>
+          <t>/r/learnpython/comments/hhu0zj/the_best_moment_ever_the_moment_when_it_finally/</t>
         </is>
       </c>
     </row>
@@ -383,7 +383,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>/r/pics/comments/hdyxvr/bubba_wallace_nascars_only_black_driver_with/</t>
+          <t>/r/pics/comments/hhydw1/oc45_years_ago_i_quit_my_stressful_desk_job_now_i/</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>/r/Python/comments/ha4qfy/whats_everyone_working_on_this_week/</t>
+          <t>/r/Python/comments/hefa1t/whats_everyone_working_on_this_week/</t>
         </is>
       </c>
     </row>

</xml_diff>